<commit_message>
new helper method added
</commit_message>
<xml_diff>
--- a/Ebay/src/test/resources/test_data/test_data.xlsx
+++ b/Ebay/src/test/resources/test_data/test_data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>First Name</t>
   </si>
@@ -317,8 +317,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="24.0" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>